<commit_message>
Removed some colukmns and wrote data to two files: df_data_X.csv and df_data_y.csv
</commit_message>
<xml_diff>
--- a/Aerodynamic-Data/Runlog.xlsx
+++ b/Aerodynamic-Data/Runlog.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John Wylie\Documents\RPI\Courses\MANE 6962 Machine Learning\Project Git\wind-turbine-regression\Aerodynamic-Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17944D7-9276-4FC4-A1C1-8A953ED27488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="255" windowWidth="17715" windowHeight="9600"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Export Mode" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="68">
   <si>
     <t>3M</t>
   </si>
@@ -241,11 +248,14 @@
   <si>
     <t>N63418-p3wrapP80_4%</t>
   </si>
+  <si>
+    <t>FileNo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1140,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1151,26 +1161,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1200,37 +1203,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1239,10 +1230,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1257,266 +1248,254 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="39" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="40" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="62" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1528,12 +1507,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1575,7 +1557,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1608,9 +1590,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1643,6 +1642,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1818,17 +1834,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
@@ -1839,10 +1855,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="97" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="111" t="s">
@@ -1852,544 +1868,544 @@
       <c r="E1" s="112"/>
       <c r="F1" s="112"/>
       <c r="G1" s="113"/>
-      <c r="H1" s="114" t="s">
+      <c r="H1" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="115" t="s">
+      <c r="I1" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="116" t="s">
+      <c r="J1" s="100" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="118"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="81" t="s">
+      <c r="A2" s="102"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="114" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="81" t="s">
+      <c r="E2" s="115"/>
+      <c r="F2" s="114" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="82"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="32" t="s">
+      <c r="G2" s="115"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="95"/>
+      <c r="J2" s="82"/>
     </row>
     <row r="3" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="119"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="36" t="s">
+      <c r="A3" s="103"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="96"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="83"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="120">
+      <c r="A4" s="104">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="D4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="J4" s="97" t="s">
+      <c r="J4" s="84" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="121">
+      <c r="A5" s="105">
         <v>2</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="23" t="s">
+      <c r="D5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="98" t="s">
+      <c r="J5" s="85" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="122">
+      <c r="A6" s="106">
         <v>3</v>
       </c>
-      <c r="B6" s="85" t="s">
+      <c r="B6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="87" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="88" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="89" t="s">
+      <c r="D6" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="90" t="s">
+      <c r="I6" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="99" t="s">
+      <c r="J6" s="86" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="123">
-        <v>4</v>
-      </c>
-      <c r="B7" s="29" t="s">
+      <c r="A7" s="107">
+        <v>4</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="83">
-        <v>0.08</v>
-      </c>
-      <c r="G7" s="84">
-        <v>0.08</v>
-      </c>
-      <c r="H7" s="31" t="s">
+      <c r="D7" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="G7" s="72">
+        <v>0.08</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="I7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="100" t="s">
+      <c r="J7" s="87" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="124">
+      <c r="A8" s="108">
         <v>5</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="92" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="92" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="93">
-        <v>0.08</v>
-      </c>
-      <c r="G8" s="94">
-        <v>0.08</v>
-      </c>
-      <c r="H8" s="89" t="s">
+      <c r="D8" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="80">
+        <v>0.08</v>
+      </c>
+      <c r="G8" s="81">
+        <v>0.08</v>
+      </c>
+      <c r="H8" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="90"/>
-      <c r="J8" s="99" t="s">
+      <c r="I8" s="77"/>
+      <c r="J8" s="86" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="125">
+      <c r="A9" s="109">
         <v>6</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="35">
         <v>40</v>
       </c>
-      <c r="E9" s="43">
+      <c r="E9" s="36">
         <v>425</v>
       </c>
-      <c r="F9" s="50">
-        <v>0.08</v>
-      </c>
-      <c r="G9" s="51">
-        <v>0.08</v>
-      </c>
-      <c r="H9" s="27" t="s">
+      <c r="F9" s="41">
+        <v>0.08</v>
+      </c>
+      <c r="G9" s="42">
+        <v>0.08</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="101" t="s">
+      <c r="J9" s="88" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="125"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="101" t="s">
+      <c r="A10" s="109"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="88" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="106">
+      <c r="A11" s="93">
         <v>7</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="33">
         <v>40</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="33">
         <v>425</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="55">
         <v>0.15</v>
       </c>
-      <c r="G11" s="66">
+      <c r="G11" s="56">
         <v>0.15</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="98" t="s">
+      <c r="J11" s="85" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="125">
+      <c r="A12" s="109">
         <v>8</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="35">
         <v>240</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="36">
         <v>53</v>
       </c>
-      <c r="F12" s="50">
+      <c r="F12" s="41">
         <v>0.04</v>
       </c>
-      <c r="G12" s="51">
+      <c r="G12" s="42">
         <v>0.04</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="101" t="s">
+      <c r="J12" s="88" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="125"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="101" t="s">
+      <c r="A13" s="109"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="88" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="126">
+      <c r="A14" s="110">
         <v>9</v>
       </c>
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="44">
+      <c r="D14" s="37">
         <v>240</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="38">
         <v>53</v>
       </c>
-      <c r="F14" s="52">
-        <v>0.08</v>
-      </c>
-      <c r="G14" s="53">
-        <v>0.08</v>
-      </c>
-      <c r="H14" s="35" t="s">
+      <c r="F14" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="G14" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="H14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="I14" s="33" t="s">
+      <c r="I14" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="J14" s="102" t="s">
+      <c r="J14" s="89" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="106">
+      <c r="A15" s="93">
         <v>10</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="44">
+      <c r="D15" s="37">
         <v>240</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="38">
         <v>53</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="43">
         <v>0.15</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="44">
         <v>0.15</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="98" t="s">
+      <c r="J15" s="85" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="106">
+      <c r="A16" s="93">
         <v>11</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="44">
+      <c r="D16" s="37">
         <v>80</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="38">
         <v>190</v>
       </c>
-      <c r="F16" s="52">
-        <v>0.08</v>
-      </c>
-      <c r="G16" s="53">
-        <v>0.08</v>
-      </c>
-      <c r="H16" s="23" t="s">
+      <c r="F16" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="G16" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="98" t="s">
+      <c r="J16" s="85" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="106">
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="93">
         <v>12</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="46">
+      <c r="D17" s="39">
         <v>80</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="40">
         <v>190</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="45">
         <v>0.15</v>
       </c>
-      <c r="G17" s="55">
+      <c r="G17" s="46">
         <v>0.15</v>
       </c>
-      <c r="H17" s="31" t="s">
+      <c r="H17" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="100" t="s">
+      <c r="J17" s="87" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="107">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="94">
         <v>13</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="69">
+      <c r="D18" s="59">
         <v>80</v>
       </c>
-      <c r="E18" s="70">
+      <c r="E18" s="60">
         <v>190</v>
       </c>
-      <c r="F18" s="71">
+      <c r="F18" s="61">
         <v>0.04</v>
       </c>
-      <c r="G18" s="72">
+      <c r="G18" s="62">
         <v>0.04</v>
       </c>
-      <c r="H18" s="73" t="s">
+      <c r="H18" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="74" t="s">
+      <c r="I18" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="103" t="s">
+      <c r="J18" s="90" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="108"/>
-      <c r="B19" s="75"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="80"/>
-      <c r="J19" s="104" t="s">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="95"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="91" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="106">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="93">
         <v>14</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="44">
+      <c r="D20" s="37">
         <v>40</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="38">
         <v>425</v>
       </c>
-      <c r="F20" s="52">
+      <c r="F20" s="43">
         <v>0.04</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="44">
         <v>0.04</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="98" t="s">
+      <c r="J20" s="85" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="106">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="93">
         <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -2398,30 +2414,30 @@
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="37">
         <v>240</v>
       </c>
-      <c r="E21" s="49">
+      <c r="E21" s="38">
         <v>53</v>
       </c>
-      <c r="F21" s="52">
-        <v>0.08</v>
-      </c>
-      <c r="G21" s="53">
+      <c r="F21" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="G21" s="44">
         <v>0.08</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J21" s="98" t="s">
+      <c r="J21" s="85" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="106">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="93">
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2430,30 +2446,30 @@
       <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="48">
+      <c r="D22" s="37">
         <v>240</v>
       </c>
-      <c r="E22" s="49">
+      <c r="E22" s="38">
         <v>53</v>
       </c>
-      <c r="F22" s="52">
-        <v>0.08</v>
-      </c>
-      <c r="G22" s="53">
+      <c r="F22" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="G22" s="44">
         <v>0.08</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="98" t="s">
+      <c r="J22" s="85" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="106">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="93">
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2462,127 +2478,100 @@
       <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="48">
+      <c r="D23" s="37">
         <v>240</v>
       </c>
-      <c r="E23" s="49">
+      <c r="E23" s="38">
         <v>53</v>
       </c>
-      <c r="F23" s="52">
-        <v>0.08</v>
-      </c>
-      <c r="G23" s="53">
+      <c r="F23" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="G23" s="44">
         <v>0.08</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="J23" s="98" t="s">
+      <c r="J23" s="85" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="109">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="96">
         <v>18</v>
       </c>
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="59">
+      <c r="D24" s="49">
         <v>80</v>
       </c>
-      <c r="E24" s="60">
+      <c r="E24" s="50">
         <v>190</v>
       </c>
-      <c r="F24" s="61">
+      <c r="F24" s="51">
         <v>0.15</v>
       </c>
-      <c r="G24" s="62">
+      <c r="G24" s="52">
         <v>0.04</v>
       </c>
-      <c r="H24" s="63" t="s">
+      <c r="H24" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="64" t="s">
+      <c r="I24" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="105" t="s">
+      <c r="J24" s="92" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="8" t="s">
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="8" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2593,4 +2582,363 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BC10CD-A8E8-448C-8ED1-EBA7F185F339}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="104">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="105">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="106">
+        <v>3</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="107">
+        <v>4</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="71">
+        <v>0.08</v>
+      </c>
+      <c r="E5" s="72">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="108">
+        <v>5</v>
+      </c>
+      <c r="B6" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="80">
+        <v>0.08</v>
+      </c>
+      <c r="E6" s="81">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="109">
+        <v>6</v>
+      </c>
+      <c r="B7" s="35">
+        <v>40</v>
+      </c>
+      <c r="C7" s="36">
+        <v>425</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0.08</v>
+      </c>
+      <c r="E7" s="42">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="109"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="93">
+        <v>7</v>
+      </c>
+      <c r="B9" s="33">
+        <v>40</v>
+      </c>
+      <c r="C9" s="33">
+        <v>425</v>
+      </c>
+      <c r="D9" s="55">
+        <v>0.15</v>
+      </c>
+      <c r="E9" s="56">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="109">
+        <v>8</v>
+      </c>
+      <c r="B10" s="35">
+        <v>240</v>
+      </c>
+      <c r="C10" s="36">
+        <v>53</v>
+      </c>
+      <c r="D10" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="E10" s="42">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="109"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="110">
+        <v>9</v>
+      </c>
+      <c r="B12" s="37">
+        <v>240</v>
+      </c>
+      <c r="C12" s="38">
+        <v>53</v>
+      </c>
+      <c r="D12" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="E12" s="44">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="93">
+        <v>10</v>
+      </c>
+      <c r="B13" s="37">
+        <v>240</v>
+      </c>
+      <c r="C13" s="38">
+        <v>53</v>
+      </c>
+      <c r="D13" s="43">
+        <v>0.15</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="93">
+        <v>11</v>
+      </c>
+      <c r="B14" s="37">
+        <v>80</v>
+      </c>
+      <c r="C14" s="38">
+        <v>190</v>
+      </c>
+      <c r="D14" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="E14" s="44">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="93">
+        <v>12</v>
+      </c>
+      <c r="B15" s="39">
+        <v>80</v>
+      </c>
+      <c r="C15" s="40">
+        <v>190</v>
+      </c>
+      <c r="D15" s="45">
+        <v>0.15</v>
+      </c>
+      <c r="E15" s="46">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="94">
+        <v>13</v>
+      </c>
+      <c r="B16" s="59">
+        <v>80</v>
+      </c>
+      <c r="C16" s="60">
+        <v>190</v>
+      </c>
+      <c r="D16" s="61">
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="62">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="95"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="46"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="93">
+        <v>14</v>
+      </c>
+      <c r="B18" s="37">
+        <v>40</v>
+      </c>
+      <c r="C18" s="38">
+        <v>425</v>
+      </c>
+      <c r="D18" s="43">
+        <v>0.04</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="93">
+        <v>15</v>
+      </c>
+      <c r="B19" s="37">
+        <v>240</v>
+      </c>
+      <c r="C19" s="38">
+        <v>53</v>
+      </c>
+      <c r="D19" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="E19" s="44">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="93">
+        <v>16</v>
+      </c>
+      <c r="B20" s="37">
+        <v>240</v>
+      </c>
+      <c r="C20" s="38">
+        <v>53</v>
+      </c>
+      <c r="D20" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="E20" s="44">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="93">
+        <v>17</v>
+      </c>
+      <c r="B21" s="37">
+        <v>240</v>
+      </c>
+      <c r="C21" s="38">
+        <v>53</v>
+      </c>
+      <c r="D21" s="43">
+        <v>0.08</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="96">
+        <v>18</v>
+      </c>
+      <c r="B22" s="49">
+        <v>80</v>
+      </c>
+      <c r="C22" s="50">
+        <v>190</v>
+      </c>
+      <c r="D22" s="51">
+        <v>0.15</v>
+      </c>
+      <c r="E22" s="52">
+        <v>0.04</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>